<commit_message>
Implementation in PublicPerson with fields Country and Country_code
</commit_message>
<xml_diff>
--- a/data/Picture/DataAngelman.xlsx
+++ b/data/Picture/DataAngelman.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\angelmanDataExtract\data\Picture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070C727E-2803-47E0-953C-8B663D584F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C75E65-4D88-47C5-B441-2D248B60647C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Id</t>
   </si>
@@ -154,48 +154,6 @@
   </si>
   <si>
     <t>Latitude</t>
-  </si>
-  <si>
-    <t>48.833328</t>
-  </si>
-  <si>
-    <t>2.25</t>
-  </si>
-  <si>
-    <t>48.829567</t>
-  </si>
-  <si>
-    <t>2.323963</t>
-  </si>
-  <si>
-    <t>48.8618779</t>
-  </si>
-  <si>
-    <t>2.3374139</t>
-  </si>
-  <si>
-    <t>48.8676828</t>
-  </si>
-  <si>
-    <t>2.3431278</t>
-  </si>
-  <si>
-    <t>43.3246669</t>
-  </si>
-  <si>
-    <t>5.4112812</t>
-  </si>
-  <si>
-    <t>43.3070787</t>
-  </si>
-  <si>
-    <t>5.3842697</t>
-  </si>
-  <si>
-    <t>43.1257311</t>
-  </si>
-  <si>
-    <t>5.9304919</t>
   </si>
   <si>
     <t>Délétion</t>
@@ -262,6 +220,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -314,19 +275,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte 2" xfId="2" xr:uid="{9451B193-6CA3-492C-A190-6484A63BB54C}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,7 +572,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H2" sqref="H2:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,6 +580,7 @@
     <col min="4" max="4" width="22.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -648,13 +613,13 @@
         <v>41</v>
       </c>
       <c r="J1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -674,25 +639,25 @@
         <v>42579</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>44</v>
+      <c r="H2" s="3">
+        <v>40.712800000000001</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-74.006</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -717,20 +682,20 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" t="s">
-        <v>48</v>
+      <c r="H3" s="4">
+        <v>34.052199999999999</v>
+      </c>
+      <c r="I3" s="4">
+        <v>-118.2437</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -755,20 +720,20 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="4">
+        <v>48.8566</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2.3521999999999998</v>
+      </c>
+      <c r="J4" t="s">
         <v>47</v>
-      </c>
-      <c r="I4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" t="s">
-        <v>61</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -788,25 +753,25 @@
         <v>43081</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" t="s">
-        <v>50</v>
+      <c r="H5" s="4">
+        <v>43.296500000000002</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5.3697999999999997</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -826,25 +791,25 @@
         <v>43687</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>46</v>
+      <c r="H6" s="5">
+        <v>40.416800000000002</v>
+      </c>
+      <c r="I6" s="5">
+        <v>-3.7038000000000002</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="K6">
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -864,25 +829,25 @@
         <v>43293</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" t="s">
-        <v>52</v>
+      <c r="H7" s="4">
+        <v>41.385100000000001</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2.1734</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="K7">
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -907,20 +872,20 @@
       <c r="G8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" t="s">
-        <v>54</v>
+      <c r="H8" s="4">
+        <v>-23.5505</v>
+      </c>
+      <c r="I8" s="4">
+        <v>-46.633299999999998</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -940,25 +905,25 @@
         <v>43831</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
         <v>36</v>
       </c>
-      <c r="H9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" t="s">
-        <v>56</v>
+      <c r="H9" s="4">
+        <v>-22.9068</v>
+      </c>
+      <c r="I9" s="4">
+        <v>-43.172899999999998</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="K9">
         <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prise en compte des langues dans la creation des conversations
</commit_message>
<xml_diff>
--- a/data/Picture/DataAngelman.xlsx
+++ b/data/Picture/DataAngelman.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\angelmanDataExtract\data\Picture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C75E65-4D88-47C5-B441-2D248B60647C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4E3C4B-8ED4-44D5-8EA3-F99B3DF2179D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t>Id</t>
   </si>
@@ -214,6 +214,27 @@
   </si>
   <si>
     <t>ReponseSecrete</t>
+  </si>
+  <si>
+    <t>IsInfo</t>
+  </si>
+  <si>
+    <t>Lang</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -221,7 +242,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -284,9 +305,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -569,374 +590,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>62</v>
       </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>42579</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>40.712800000000001</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>-74.006</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>54</v>
       </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>36939</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>34.052199999999999</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>-118.2437</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>46</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>55</v>
       </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>40430</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>48.8566</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>2.3521999999999998</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>47</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>3</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>56</v>
       </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>43081</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>43.296500000000002</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>5.3697999999999997</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>48</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>57</v>
       </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>43687</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>43</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>40.416800000000002</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>-3.7038000000000002</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>49</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>2</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>58</v>
       </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>43293</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="4">
         <v>41.385100000000001</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>2.1734</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>50</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>59</v>
       </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>42837</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>-23.5505</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="4">
         <v>-46.633299999999998</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>60</v>
       </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>43831</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>43</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>-22.9068</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <v>-43.172899999999998</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>52</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>2</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>61</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{1C8E9A43-53CF-4F5E-B3F0-5A02810E80EB}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{F8A96644-F00D-4D54-8AAD-6F54AADC842D}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{218BD25C-C5C4-47DA-B773-5C4D9AC59C16}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{03526046-7F31-48C4-A188-A7633751D8A8}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{C1C5F56B-E83A-4B4E-A7DE-ED45E42A76B2}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{CED7B535-2CF7-48BE-8F20-73B0E9DBC149}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{E2D57572-4AE6-4CC7-B825-120EB420675E}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{825DF4FD-3B3C-4C9E-A0E0-94733C682596}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1C8E9A43-53CF-4F5E-B3F0-5A02810E80EB}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{F8A96644-F00D-4D54-8AAD-6F54AADC842D}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{218BD25C-C5C4-47DA-B773-5C4D9AC59C16}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{03526046-7F31-48C4-A188-A7633751D8A8}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{C1C5F56B-E83A-4B4E-A7DE-ED45E42A76B2}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{CED7B535-2CF7-48BE-8F20-73B0E9DBC149}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{E2D57572-4AE6-4CC7-B825-120EB420675E}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{825DF4FD-3B3C-4C9E-A0E0-94733C682596}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>